<commit_message>
Updated Settings with Orchestrator name , System1 URL and Credentials
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="396" yWindow="480" windowWidth="10236" windowHeight="7620"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Settings" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Constants" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Assets" sheetId="3" r:id="rId5"/>
+    <sheet name="Settings" sheetId="1" r:id="rId1"/>
+    <sheet name="Constants" sheetId="2" r:id="rId2"/>
+    <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -147,9 +150,6 @@
     <t>OrchestratorQueueName</t>
   </si>
   <si>
-    <t>KibanaDemoQueue</t>
-  </si>
-  <si>
     <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
   </si>
   <si>
@@ -160,21 +160,33 @@
   </si>
   <si>
     <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
+  </si>
+  <si>
+    <t>ACME_URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
+  </si>
+  <si>
+    <t>ACME_Credentials</t>
+  </si>
+  <si>
+    <t>InHouse_Process4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="2">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -184,54 +196,334 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="68.0"/>
-    <col customWidth="1" min="2" max="2" width="70.14"/>
-    <col customWidth="1" min="3" max="3" width="68.57"/>
-    <col customWidth="1" min="4" max="26" width="8.71"/>
+    <col min="1" max="1" width="68" customWidth="1"/>
+    <col min="2" max="2" width="70.109375" customWidth="1"/>
+    <col min="3" max="3" width="68.5546875" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -265,41 +557,55 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
         <v>45</v>
       </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1"/>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
         <v>48</v>
       </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1282,24 +1588,25 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="53.0"/>
-    <col customWidth="1" min="2" max="2" width="63.57"/>
-    <col customWidth="1" min="3" max="3" width="89.0"/>
-    <col customWidth="1" min="4" max="26" width="8.71"/>
+    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
+    <col min="3" max="3" width="89" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1333,54 +1640,54 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>5000.0</v>
+        <v>5000</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
-        <v>30000.0</v>
+        <v>30000</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7">
-        <v>120000.0</v>
+        <v>120000</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1391,42 +1698,42 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12">
-        <v>15000.0</v>
+        <v>15000</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13">
-        <v>60000.0</v>
+        <v>60000</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1437,7 +1744,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1448,7 +1755,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1459,8 +1766,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1">
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1471,7 +1778,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1482,7 +1789,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1493,7 +1800,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1504,7 +1811,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1515,15 +1822,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2493,21 +2800,22 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="65.43"/>
+    <col min="1" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2541,21 +2849,21 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1"/>
-    <row r="3" ht="14.25" customHeight="1"/>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1"/>
-    <row r="6" ht="14.25" customHeight="1"/>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
-    <row r="12" ht="14.25" customHeight="1"/>
-    <row r="13" ht="14.25" customHeight="1"/>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1"/>
-    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -3541,6 +3849,6 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Navigation to download monthly report
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>InHouse_Process4</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Temporay Folder to download monthly report</t>
   </si>
 </sst>
 </file>
@@ -512,7 +518,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -596,7 +602,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Created cleanup workflow to delete and create temporary folder to download monthly reports
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Temporay Folder to download monthly report</t>
+  </si>
+  <si>
+    <t>Data\Temp</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -607,7 +610,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Generate Yearly Report Finished
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>Data\Temp</t>
+  </si>
+  <si>
+    <t>YearReport</t>
+  </si>
+  <si>
+    <t>Data\YearReport</t>
+  </si>
+  <si>
+    <t>Folder to collect Yearly repot</t>
   </si>
 </sst>
 </file>
@@ -521,7 +530,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -616,7 +625,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>